<commit_message>
Ultima entrega de BFIN
</commit_message>
<xml_diff>
--- a/B2-1/BFIN/Actividades/BFIN_U5_EA_BERC.xlsx
+++ b/B2-1/BFIN/Actividades/BFIN_U5_EA_BERC.xlsx
@@ -17,7 +17,7 @@
     <definedName function="false" hidden="false" name="PercentComplete" vbProcedure="false">PercentCompleteBeyond*PeriodInPlan</definedName>
     <definedName function="false" hidden="false" name="PercentCompleteBeyond" vbProcedure="false">('Planificador de proyectos'!A$4=MEDIAN('Planificador de proyectos'!A$4,'Planificador de proyectos'!$E1,'Planificador de proyectos'!$E1+'Planificador de proyectos'!$F1)*('Planificador de proyectos'!$E1&gt;0))*(('Planificador de proyectos'!A$4&lt;(INT('Planificador de proyectos'!$E1+'Planificador de proyectos'!$F1*'Planificador de proyectos'!$G1)))+('Planificador de proyectos'!A$4='Planificador de proyectos'!$E1))*('Planificador de proyectos'!$G1&gt;0)</definedName>
     <definedName function="false" hidden="false" name="PeriodInPlan" vbProcedure="false">'Planificador de proyectos'!A$4=MEDIAN('Planificador de proyectos'!A$4,'Planificador de proyectos'!$C1,'Planificador de proyectos'!$C1+'Planificador de proyectos'!$D1-1)</definedName>
-    <definedName function="false" hidden="false" name="period_selected" vbProcedure="false">'Planificador de proyectos'!$H$2</definedName>
+    <definedName function="false" hidden="false" name="period_selected" vbProcedure="false">'Planificador de proyectos'!$C$2</definedName>
     <definedName function="false" hidden="false" name="Plan" vbProcedure="false">PeriodInPlan*('Planificador de proyectos'!$C1&gt;0)</definedName>
     <definedName function="false" hidden="false" name="Real" vbProcedure="false">(PeriodInActual*('Planificador de proyectos'!$E1&gt;0))*PeriodInPlan</definedName>
     <definedName function="false" hidden="false" name="TitleRegion..BO60" vbProcedure="false">'Planificador de proyectos'!$B$3:$B$4</definedName>
@@ -32,12 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">Planificador de proyectos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selecciona un período para resaltarlo a la derecha.  A continuación hay una leyenda que describe el gráfico.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+  <si>
+    <t xml:space="preserve">Mi proyecto de investigación</t>
   </si>
   <si>
     <t xml:space="preserve"> Período resaltado:</t>
@@ -156,6 +153,22 @@
     <t xml:space="preserve">PERÍODOS</t>
   </si>
   <si>
+    <t xml:space="preserve">EA Parte 1
+Objetivos y justificación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EA Parte 2
+Marco Teórico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EA Parte 3
+Alcance e instrumentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EA Parte 4
+Software y cronográma</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajuste y planeación del proyecto</t>
   </si>
   <si>
@@ -180,7 +193,7 @@
     <t xml:space="preserve">Análisis de datos recopilados</t>
   </si>
   <si>
-    <t xml:space="preserve">Segunda vuelta de aplicacion de encuestas y experimentos</t>
+    <t xml:space="preserve">Segunda vuelta de encuestas y experimentos</t>
   </si>
   <si>
     <t xml:space="preserve">Elaboración de reporte</t>
@@ -202,7 +215,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
@@ -280,14 +293,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF735773"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
@@ -296,7 +301,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="13"/>
+      <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -354,7 +359,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -443,8 +448,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="38">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,9 +528,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
@@ -529,7 +538,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,67 +563,63 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="2" xfId="31" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="2" xfId="31" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="29" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="27" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="35" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="37" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -630,16 +635,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -660,10 +665,9 @@
     <cellStyle name="Valor del período" xfId="31"/>
     <cellStyle name="Excel Built-in Title" xfId="32"/>
     <cellStyle name="Excel Built-in Heading 1" xfId="33"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="34"/>
-    <cellStyle name="Excel Built-in Heading 2" xfId="35"/>
-    <cellStyle name="Excel Built-in Heading 3" xfId="36"/>
-    <cellStyle name="Excel Built-in Heading 4" xfId="37"/>
+    <cellStyle name="Excel Built-in Heading 2" xfId="34"/>
+    <cellStyle name="Excel Built-in Heading 3" xfId="35"/>
+    <cellStyle name="Excel Built-in Heading 4" xfId="36"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -873,20 +877,23 @@
   </sheetPr>
   <dimension ref="B1:BO1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE22" activeCellId="0" sqref="A1:AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="13.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="8" style="2" width="2.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -896,555 +903,638 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+    <row r="2" s="6" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="12" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="14" t="s">
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="10" t="s">
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="14" t="s">
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+    </row>
+    <row r="3" s="16" customFormat="true" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
-      <c r="AR2" s="14"/>
-      <c r="AS2" s="14"/>
-      <c r="AT2" s="14"/>
-    </row>
-    <row r="3" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="M4" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="N4" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="O4" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="P4" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="R4" s="23" t="n">
+        <v>11</v>
+      </c>
+      <c r="S4" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="T4" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="U4" s="23" t="n">
         <v>14</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="24" t="n">
+      <c r="V4" s="23" t="n">
+        <v>15</v>
+      </c>
+      <c r="W4" s="23" t="n">
+        <v>16</v>
+      </c>
+      <c r="X4" s="23" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="23" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="23" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="23" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="23" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC4" s="23" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="23" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="23" t="n">
+        <v>24</v>
+      </c>
+      <c r="AF4" s="23" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG4" s="23" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH4" s="23" t="n">
+        <v>27</v>
+      </c>
+      <c r="AI4" s="23" t="n">
+        <v>28</v>
+      </c>
+      <c r="AJ4" s="23" t="n">
+        <v>29</v>
+      </c>
+      <c r="AK4" s="23" t="n">
+        <v>30</v>
+      </c>
+      <c r="AL4" s="23" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM4" s="23" t="n">
+        <v>32</v>
+      </c>
+      <c r="AN4" s="23" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO4" s="23" t="n">
+        <v>34</v>
+      </c>
+      <c r="AP4" s="23" t="n">
+        <v>35</v>
+      </c>
+      <c r="AQ4" s="23" t="n">
+        <v>36</v>
+      </c>
+      <c r="AR4" s="23" t="n">
+        <v>37</v>
+      </c>
+      <c r="AS4" s="23" t="n">
+        <v>38</v>
+      </c>
+      <c r="AT4" s="23" t="n">
+        <v>39</v>
+      </c>
+      <c r="AU4" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="AV4" s="23" t="n">
+        <v>41</v>
+      </c>
+      <c r="AW4" s="23" t="n">
+        <v>42</v>
+      </c>
+      <c r="AX4" s="23" t="n">
+        <v>43</v>
+      </c>
+      <c r="AY4" s="23" t="n">
+        <v>44</v>
+      </c>
+      <c r="AZ4" s="23" t="n">
+        <v>45</v>
+      </c>
+      <c r="BA4" s="23" t="n">
+        <v>46</v>
+      </c>
+      <c r="BB4" s="23" t="n">
+        <v>47</v>
+      </c>
+      <c r="BC4" s="23" t="n">
+        <v>48</v>
+      </c>
+      <c r="BD4" s="23" t="n">
+        <v>49</v>
+      </c>
+      <c r="BE4" s="23" t="n">
+        <v>50</v>
+      </c>
+      <c r="BF4" s="23" t="n">
+        <v>51</v>
+      </c>
+      <c r="BG4" s="23" t="n">
+        <v>52</v>
+      </c>
+      <c r="BH4" s="23" t="n">
+        <v>53</v>
+      </c>
+      <c r="BI4" s="23" t="n">
+        <v>54</v>
+      </c>
+      <c r="BJ4" s="23" t="n">
+        <v>55</v>
+      </c>
+      <c r="BK4" s="23" t="n">
+        <v>56</v>
+      </c>
+      <c r="BL4" s="23" t="n">
+        <v>57</v>
+      </c>
+      <c r="BM4" s="23" t="n">
+        <v>58</v>
+      </c>
+      <c r="BN4" s="23" t="n">
+        <v>59</v>
+      </c>
+      <c r="BO4" s="23" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="D6" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="D7" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="L4" s="24" t="n">
+      <c r="D8" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="25" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="25" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="25" t="n">
+        <v>11</v>
+      </c>
+      <c r="D16" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="25" t="n">
+        <v>12</v>
+      </c>
+      <c r="D17" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="25" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="25" t="n">
+        <v>17</v>
+      </c>
+      <c r="D20" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="M4" s="24" t="n">
-        <v>6</v>
-      </c>
-      <c r="N4" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O4" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="P4" s="24" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="R4" s="24" t="n">
-        <v>11</v>
-      </c>
-      <c r="S4" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="T4" s="24" t="n">
-        <v>13</v>
-      </c>
-      <c r="U4" s="24" t="n">
-        <v>14</v>
-      </c>
-      <c r="V4" s="24" t="n">
-        <v>15</v>
-      </c>
-      <c r="W4" s="24" t="n">
-        <v>16</v>
-      </c>
-      <c r="X4" s="24" t="n">
-        <v>17</v>
-      </c>
-      <c r="Y4" s="24" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z4" s="24" t="n">
+      <c r="E20" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="25" t="n">
         <v>19</v>
       </c>
-      <c r="AA4" s="24" t="n">
-        <v>20</v>
-      </c>
-      <c r="AB4" s="24" t="n">
-        <v>21</v>
-      </c>
-      <c r="AC4" s="24" t="n">
+      <c r="D21" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="25" t="n">
         <v>22</v>
       </c>
-      <c r="AD4" s="24" t="n">
-        <v>23</v>
-      </c>
-      <c r="AE4" s="24" t="n">
-        <v>24</v>
-      </c>
-      <c r="AF4" s="24" t="n">
-        <v>25</v>
-      </c>
-      <c r="AG4" s="24" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH4" s="24" t="n">
-        <v>27</v>
-      </c>
-      <c r="AI4" s="24" t="n">
-        <v>28</v>
-      </c>
-      <c r="AJ4" s="24" t="n">
-        <v>29</v>
-      </c>
-      <c r="AK4" s="24" t="n">
-        <v>30</v>
-      </c>
-      <c r="AL4" s="24" t="n">
-        <v>31</v>
-      </c>
-      <c r="AM4" s="24" t="n">
-        <v>32</v>
-      </c>
-      <c r="AN4" s="24" t="n">
-        <v>33</v>
-      </c>
-      <c r="AO4" s="24" t="n">
-        <v>34</v>
-      </c>
-      <c r="AP4" s="24" t="n">
-        <v>35</v>
-      </c>
-      <c r="AQ4" s="24" t="n">
-        <v>36</v>
-      </c>
-      <c r="AR4" s="24" t="n">
-        <v>37</v>
-      </c>
-      <c r="AS4" s="24" t="n">
-        <v>38</v>
-      </c>
-      <c r="AT4" s="24" t="n">
-        <v>39</v>
-      </c>
-      <c r="AU4" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="24" t="n">
-        <v>41</v>
-      </c>
-      <c r="AW4" s="24" t="n">
-        <v>42</v>
-      </c>
-      <c r="AX4" s="24" t="n">
-        <v>43</v>
-      </c>
-      <c r="AY4" s="24" t="n">
-        <v>44</v>
-      </c>
-      <c r="AZ4" s="24" t="n">
-        <v>45</v>
-      </c>
-      <c r="BA4" s="24" t="n">
-        <v>46</v>
-      </c>
-      <c r="BB4" s="24" t="n">
-        <v>47</v>
-      </c>
-      <c r="BC4" s="24" t="n">
-        <v>48</v>
-      </c>
-      <c r="BD4" s="24" t="n">
-        <v>49</v>
-      </c>
-      <c r="BE4" s="24" t="n">
-        <v>50</v>
-      </c>
-      <c r="BF4" s="24" t="n">
-        <v>51</v>
-      </c>
-      <c r="BG4" s="24" t="n">
-        <v>52</v>
-      </c>
-      <c r="BH4" s="24" t="n">
-        <v>53</v>
-      </c>
-      <c r="BI4" s="24" t="n">
-        <v>54</v>
-      </c>
-      <c r="BJ4" s="24" t="n">
-        <v>55</v>
-      </c>
-      <c r="BK4" s="24" t="n">
-        <v>56</v>
-      </c>
-      <c r="BL4" s="24" t="n">
-        <v>57</v>
-      </c>
-      <c r="BM4" s="24" t="n">
-        <v>58</v>
-      </c>
-      <c r="BN4" s="24" t="n">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="24" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E10" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="26" t="n">
-        <v>9</v>
-      </c>
-      <c r="D11" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="26" t="n">
-        <v>11</v>
-      </c>
-      <c r="D13" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="26" t="n">
-        <v>13</v>
-      </c>
-      <c r="D14" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="E14" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="26" t="n">
-        <v>15</v>
-      </c>
-      <c r="D15" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="E15" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="26" t="n">
-        <v>17</v>
-      </c>
-      <c r="D16" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="D17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="n">
+      <c r="D22" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1462,13 +1552,12 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="AC2:AI2"/>
-    <mergeCell ref="AK2:AT2"/>
+  <mergeCells count="11">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="AA2:AJ2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -1476,7 +1565,7 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO17">
+  <conditionalFormatting sqref="H5:BO9 AQ10:BO17 H10:AP22">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1502,7 +1591,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:BO18">
+  <conditionalFormatting sqref="AQ18:BO18">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>1</formula>
     </cfRule>
@@ -1512,32 +1601,32 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="between" prompt="El planificador de proyectos usa períodos para los intervalos. Inicio = 1 es el período 1 y la duración = 5 significa que el proyecto dura 5 períodos desde el período de inicio. Introduce datos a partir de la celda B5 para actualizar el gráfico." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Escribe un valor del 1 al 60 o selecciona un período de la lista (presiona CANCELAR, ALT+FLECHA ABAJO y, a continuación, presiona ENTRAR para seleccionar un valor)." operator="between" prompt="Escribe un período en el intervalo de 1 a 60 o selecciona un período de la lista. Presiona ALT+FLECHA ABAJO para desplazarse a la lista y, después, presiona ENTRAR para seleccionar un valor." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2" type="list">
+    <dataValidation allowBlank="true" error="Escribe un valor del 1 al 60 o selecciona un período de la lista (presiona CANCELAR, ALT+FLECHA ABAJO y, a continuación, presiona ENTRAR para seleccionar un valor)." operator="between" prompt="Escribe un período en el intervalo de 1 a 60 o selecciona un período de la lista. Presiona ALT+FLECHA ABAJO para desplazarse a la lista y, después, presiona ENTRAR para seleccionar un valor." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2" type="list">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración real" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q2" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración real" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V2" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración real fuera del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB2" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica la duración real fuera del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado fuera del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ2" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado fuera del plan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Z2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1573,10 +1662,6 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Selecciona un período para resaltar en H2. La leyenda de un gráfico está en las celdas J2 a AI2." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:F2" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.511805555555555" footer="0.3"/>

</xml_diff>